<commit_message>
ResAssg: j721e: Fix subtype names
* Rename the sheet to j721e
* Fix subtype names

Signed-off-by: Nikhil Devshatwar <nikhil.nd@ti.com>
</commit_message>
<xml_diff>
--- a/respart/SYSFW-NAVSS-ResAssg.xlsx
+++ b/respart/SYSFW-NAVSS-ResAssg.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11988" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="j721e-evm" sheetId="4" r:id="rId1"/>
+    <sheet name="j721e" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -325,9 +325,6 @@
     <t>RESASG_SUBTYPE_R5FSS1_CORE0_INTR_IRQ_GROUP0_FROM_GPIOMUX_INTRTR0</t>
   </si>
   <si>
-    <t>RESASG_SUBTYPE_R5FSS1_CORE0_INTR_IRQ_GROUP0_FROM_NAVSS1_INTR_ROUTER_0</t>
-  </si>
-  <si>
     <t>Main R5FSS1 core0 IPI interrupt router</t>
   </si>
   <si>
@@ -343,9 +340,6 @@
     <t>RESASG_SUBTYPE_R5FSS1_CORE1_INTR_IRQ_GROUP0_FROM_GPIOMUX_INTRTR0</t>
   </si>
   <si>
-    <t>RESASG_SUBTYPE_R5FSS1_CORE1_INTR_IRQ_GROUP0_FROM_NAVSS1_INTR_ROUTER_0</t>
-  </si>
-  <si>
     <t>Main R5FSS1 core1 IPI interrupt router</t>
   </si>
   <si>
@@ -497,6 +491,12 @@
   </si>
   <si>
     <t>NAVSS interrupt router for R5FSS1 core1</t>
+  </si>
+  <si>
+    <t>RESASG_SUBTYPE_R5FSS1_CORE1_INTR_IRQ_GROUP0_FROM_NAVSS0_INTR_ROUTER_0</t>
+  </si>
+  <si>
+    <t>RESASG_SUBTYPE_R5FSS1_CORE0_INTR_IRQ_GROUP0_FROM_NAVSS0_INTR_ROUTER_0</t>
   </si>
 </sst>
 </file>
@@ -2397,10 +2397,10 @@
   <dimension ref="A1:W85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomRight" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -4663,13 +4663,13 @@
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="D43" s="15">
         <v>28</v>
@@ -4712,13 +4712,13 @@
     </row>
     <row r="44" spans="1:21">
       <c r="A44" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D44" s="15">
         <v>256</v>
@@ -4761,13 +4761,13 @@
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="C45" s="13" t="s">
         <v>101</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>102</v>
       </c>
       <c r="D45" s="15">
         <v>16</v>
@@ -4810,13 +4810,13 @@
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="D46" s="15">
         <v>28</v>
@@ -4859,13 +4859,13 @@
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D47" s="15">
         <v>256</v>
@@ -4908,13 +4908,13 @@
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="13" t="s">
         <v>106</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>108</v>
       </c>
       <c r="D48" s="15">
         <v>1</v>
@@ -4957,13 +4957,13 @@
     </row>
     <row r="49" spans="1:21">
       <c r="A49" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B49" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="13" t="s">
         <v>107</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>109</v>
       </c>
       <c r="D49" s="15">
         <v>81</v>
@@ -5006,13 +5006,13 @@
     </row>
     <row r="50" spans="1:21">
       <c r="A50" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D50" s="15">
         <v>1</v>
@@ -5055,13 +5055,13 @@
     </row>
     <row r="51" spans="1:21">
       <c r="A51" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D51" s="15">
         <v>8</v>
@@ -5104,13 +5104,13 @@
     </row>
     <row r="52" spans="1:21">
       <c r="A52" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D52" s="15">
         <v>2</v>
@@ -5153,13 +5153,13 @@
     </row>
     <row r="53" spans="1:21">
       <c r="A53" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="13" t="s">
         <v>113</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>115</v>
       </c>
       <c r="D53" s="15">
         <v>1</v>
@@ -5202,13 +5202,13 @@
     </row>
     <row r="54" spans="1:21">
       <c r="A54" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B54" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="13" t="s">
         <v>114</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>116</v>
       </c>
       <c r="D54" s="15">
         <v>81</v>
@@ -5251,13 +5251,13 @@
     </row>
     <row r="55" spans="1:21">
       <c r="A55" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D55" s="15">
         <v>1</v>
@@ -5300,13 +5300,13 @@
     </row>
     <row r="56" spans="1:21">
       <c r="A56" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D56" s="15">
         <v>8</v>
@@ -5349,13 +5349,13 @@
     </row>
     <row r="57" spans="1:21">
       <c r="A57" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D57" s="15">
         <v>2</v>
@@ -5398,13 +5398,13 @@
     </row>
     <row r="58" spans="1:21">
       <c r="A58" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="13" t="s">
         <v>120</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>122</v>
       </c>
       <c r="D58" s="15">
         <v>56</v>
@@ -5449,13 +5449,13 @@
     </row>
     <row r="59" spans="1:21">
       <c r="A59" s="21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D59" s="15">
         <v>16</v>
@@ -5498,13 +5498,13 @@
     </row>
     <row r="60" spans="1:21">
       <c r="A60" s="21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D60" s="15">
         <v>16</v>
@@ -5545,13 +5545,13 @@
     </row>
     <row r="61" spans="1:21">
       <c r="A61" s="21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D61" s="15">
         <v>64</v>
@@ -5594,13 +5594,13 @@
     </row>
     <row r="62" spans="1:21">
       <c r="A62" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" s="13" t="s">
         <v>127</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>129</v>
       </c>
       <c r="D62" s="15">
         <v>64</v>
@@ -5643,13 +5643,13 @@
     </row>
     <row r="63" spans="1:21">
       <c r="A63" s="21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D63" s="15">
         <v>64</v>
@@ -5694,7 +5694,7 @@
     </row>
     <row r="64" spans="1:21">
       <c r="A64" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
@@ -5757,7 +5757,7 @@
     </row>
     <row r="65" spans="1:21">
       <c r="A65" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
@@ -5782,10 +5782,10 @@
     </row>
     <row r="66" spans="1:21">
       <c r="A66" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>30</v>
@@ -5831,10 +5831,10 @@
     </row>
     <row r="67" spans="1:21">
       <c r="A67" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>32</v>
@@ -5930,7 +5930,7 @@
     </row>
     <row r="69" spans="1:21">
       <c r="A69" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -5982,7 +5982,7 @@
     </row>
     <row r="70" spans="1:21">
       <c r="A70" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -6034,10 +6034,10 @@
     </row>
     <row r="71" spans="1:21">
       <c r="A71" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>37</v>
@@ -6114,10 +6114,10 @@
     </row>
     <row r="72" spans="1:21">
       <c r="A72" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>39</v>
@@ -6268,10 +6268,10 @@
     </row>
     <row r="75" spans="1:21">
       <c r="A75" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>55</v>
@@ -6348,10 +6348,10 @@
     </row>
     <row r="76" spans="1:21">
       <c r="A76" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>57</v>
@@ -6428,10 +6428,10 @@
     </row>
     <row r="77" spans="1:21">
       <c r="A77" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C77" s="9" t="s">
         <v>59</v>
@@ -6508,10 +6508,10 @@
     </row>
     <row r="78" spans="1:21">
       <c r="A78" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C78" s="9" t="s">
         <v>61</v>
@@ -6588,10 +6588,10 @@
     </row>
     <row r="79" spans="1:21">
       <c r="A79" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C79" s="13" t="s">
         <v>68</v>
@@ -6657,10 +6657,10 @@
     </row>
     <row r="80" spans="1:21">
       <c r="A80" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C80" s="13" t="s">
         <v>71</v>
@@ -6731,10 +6731,10 @@
     </row>
     <row r="82" spans="1:21">
       <c r="A82" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>73</v>
@@ -6794,10 +6794,10 @@
     </row>
     <row r="83" spans="1:21">
       <c r="A83" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>66</v>
@@ -6863,10 +6863,10 @@
     </row>
     <row r="84" spans="1:21">
       <c r="A84" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C84" s="9" t="s">
         <v>76</v>
@@ -6932,10 +6932,10 @@
     </row>
     <row r="85" spans="1:21">
       <c r="A85" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C85" s="9" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
RM-autogen-data.py: Add support for am65x SR1 and SR2
Auto generate the python headers from documentation
Update the argparse to support both Silicon revisions.
Create baseline excel sheet for am6x and am65x_sr2

Signed-off-by: Nikhil Devshatwar <nikhil.nd@ti.com>
</commit_message>
<xml_diff>
--- a/respart/SYSFW-NAVSS-ResAssg.xlsx
+++ b/respart/SYSFW-NAVSS-ResAssg.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11988" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11988" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="j721e" sheetId="4" r:id="rId1"/>
+    <sheet name="am6x" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="149">
   <si>
     <t>Resource</t>
   </si>
@@ -223,24 +224,12 @@
     <t>MCU Nav High Capacity RX channel</t>
   </si>
   <si>
-    <t>MCU Nav Total TX channel</t>
-  </si>
-  <si>
-    <t>MCU Nav Total RX channel</t>
-  </si>
-  <si>
     <t>MCU Nav High Capacity Tx ring</t>
   </si>
   <si>
     <t>MCU Nav High Capacity Rx ring</t>
   </si>
   <si>
-    <t>MCU Nav Tx ring</t>
-  </si>
-  <si>
-    <t>MCU Nav Rx ring</t>
-  </si>
-  <si>
     <t>MCU Nav ring monitors</t>
   </si>
   <si>
@@ -379,9 +368,6 @@
     <t>MCU invalid flow OES</t>
   </si>
   <si>
-    <t>MCU Nav invalid flow OES</t>
-  </si>
-  <si>
     <t>Main Nav invalid flow OES</t>
   </si>
   <si>
@@ -407,6 +393,91 @@
   </si>
   <si>
     <t>Resource start</t>
+  </si>
+  <si>
+    <t>AM6_DEV_CMPEVENT_INTRTR0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_MAIN2MCU_LVL_INTRTR0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_MAIN2MCU_PLS_INTRTR0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_GPIOMUX_INTRTR0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_NAVSS0_INTR_ROUTER_0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_NAVSS0_MODSS_INTA0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_NAVSS0_MODSS_INTA1</t>
+  </si>
+  <si>
+    <t>AM6_DEV_NAVSS0_PROXY0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_NAVSS0_RINGACC0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_NAVSS0_UDMAP0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_NAVSS0_UDMASS_INTA0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_MCU_NAVSS0_INTR_ROUTER_0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_MCU_NAVSS0_PROXY0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_MCU_NAVSS0_RINGACC0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_MCU_NAVSS0_UDMAP0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_MCU_NAVSS0_INTR_AGGR_0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_TIMESYNC_INTRTR0</t>
+  </si>
+  <si>
+    <t>AM6_DEV_WKUP_GPIOMUX_INTRTR0</t>
+  </si>
+  <si>
+    <t>MCU Nav Ring Error OES</t>
+  </si>
+  <si>
+    <t>MCU Nav Normal Capacity Rx ring</t>
+  </si>
+  <si>
+    <t>MCU Nav Normal Capacity Tx ring</t>
+  </si>
+  <si>
+    <t>MCU Nav Normal Capacity RX channels</t>
+  </si>
+  <si>
+    <t>MCU Nav Normal Capacity TX channels</t>
+  </si>
+  <si>
+    <t>HOST_ID_A53_2
+(Uboot/ VM1/RTOS )</t>
+  </si>
+  <si>
+    <t>HOST_ID_A53_3
+(Linux VM2 )</t>
+  </si>
+  <si>
+    <t>HOST_ID_R5_0
+(MCUSW)</t>
+  </si>
+  <si>
+    <t>HOST_ID_R5_2
+(MCUSW)</t>
   </si>
 </sst>
 </file>
@@ -592,7 +663,721 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
+  <dxfs count="176">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDCE6F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1713,11 +2498,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1744,10 +2529,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>3</v>
@@ -1786,12 +2571,12 @@
         <v>14</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>43</v>
@@ -1825,7 +2610,7 @@
     </row>
     <row r="3" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>45</v>
@@ -1859,7 +2644,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>46</v>
@@ -1891,7 +2676,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>47</v>
@@ -1927,7 +2712,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>48</v>
@@ -1963,7 +2748,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>49</v>
@@ -1995,7 +2780,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>50</v>
@@ -2031,7 +2816,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>51</v>
@@ -2067,7 +2852,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>52</v>
@@ -2099,7 +2884,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>53</v>
@@ -2131,7 +2916,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>56</v>
@@ -2163,7 +2948,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>56</v>
@@ -2195,7 +2980,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>57</v>
@@ -2227,7 +3012,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>57</v>
@@ -2259,7 +3044,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>36</v>
@@ -2309,7 +3094,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>36</v>
@@ -2363,7 +3148,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>33</v>
@@ -2417,7 +3202,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>23</v>
@@ -2449,7 +3234,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>23</v>
@@ -2503,7 +3288,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>23</v>
@@ -2557,7 +3342,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>23</v>
@@ -2611,7 +3396,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>23</v>
@@ -2651,7 +3436,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>23</v>
@@ -2689,7 +3474,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>23</v>
@@ -2725,7 +3510,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>23</v>
@@ -2763,7 +3548,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>23</v>
@@ -2799,7 +3584,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>23</v>
@@ -2831,7 +3616,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>23</v>
@@ -2885,7 +3670,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>15</v>
@@ -2925,7 +3710,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>15</v>
@@ -2957,7 +3742,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>15</v>
@@ -2989,7 +3774,7 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>15</v>
@@ -3021,7 +3806,7 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>15</v>
@@ -3075,7 +3860,7 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>15</v>
@@ -3113,7 +3898,7 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>15</v>
@@ -3149,7 +3934,7 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>15</v>
@@ -3203,7 +3988,7 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>15</v>
@@ -3243,7 +4028,7 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>15</v>
@@ -3281,7 +4066,7 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>15</v>
@@ -3317,7 +4102,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>54</v>
@@ -3353,7 +4138,7 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>54</v>
@@ -3387,7 +4172,7 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>54</v>
@@ -3421,7 +4206,7 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>54</v>
@@ -3455,7 +4240,7 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>54</v>
@@ -3491,7 +4276,7 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>54</v>
@@ -3525,12 +4310,12 @@
         <v>0</v>
       </c>
       <c r="R46" s="11" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>54</v>
@@ -3566,12 +4351,12 @@
         <v>104</v>
       </c>
       <c r="R47" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>42</v>
@@ -3625,7 +4410,7 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>42</v>
@@ -3679,7 +4464,7 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>41</v>
@@ -3733,7 +4518,7 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>40</v>
@@ -3765,7 +4550,7 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>40</v>
@@ -3819,7 +4604,7 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>40</v>
@@ -3873,7 +4658,7 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>40</v>
@@ -3927,7 +4712,7 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>40</v>
@@ -3961,7 +4746,7 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>40</v>
@@ -3995,7 +4780,7 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>40</v>
@@ -4027,7 +4812,7 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>40</v>
@@ -4081,7 +4866,7 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>39</v>
@@ -4129,7 +4914,7 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>39</v>
@@ -4161,7 +4946,7 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>39</v>
@@ -4193,7 +4978,7 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>39</v>
@@ -4225,7 +5010,7 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>39</v>
@@ -4313,7 +5098,7 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
-        <v>65</v>
+        <v>144</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>39</v>
@@ -4401,7 +5186,7 @@
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>55</v>
@@ -4435,7 +5220,7 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>55</v>
@@ -4469,324 +5254,2258 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q26">
-    <cfRule type="cellIs" dxfId="91" priority="223" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="224" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="225" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="226" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="175" priority="223" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="174" priority="224" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="173" priority="225" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="172" priority="226" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q29">
-    <cfRule type="cellIs" dxfId="87" priority="219" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="220" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="221" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="222" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="171" priority="219" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="170" priority="220" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="169" priority="221" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="168" priority="222" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q30">
-    <cfRule type="cellIs" dxfId="83" priority="215" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="216" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="217" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="218" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="167" priority="215" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="166" priority="216" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="165" priority="217" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="218" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q50">
-    <cfRule type="cellIs" dxfId="79" priority="67" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="68" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="69" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="163" priority="67" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="162" priority="68" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="161" priority="69" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="160" priority="70" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q44">
-    <cfRule type="cellIs" dxfId="75" priority="51" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="52" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="53" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="159" priority="51" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="52" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="157" priority="53" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="156" priority="54" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q45">
-    <cfRule type="cellIs" dxfId="71" priority="55" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="56" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="57" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="155" priority="55" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="154" priority="56" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="153" priority="57" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="152" priority="58" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q47">
-    <cfRule type="cellIs" dxfId="67" priority="59" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="60" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="61" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="62" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="151" priority="59" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="60" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="149" priority="61" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="62" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q49">
-    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="64" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="65" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="66" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="147" priority="63" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="64" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="145" priority="65" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="144" priority="66" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q43">
-    <cfRule type="cellIs" dxfId="59" priority="47" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="48" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="49" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="143" priority="47" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="142" priority="48" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="49" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="140" priority="50" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q42">
-    <cfRule type="cellIs" dxfId="55" priority="43" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="44" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="45" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="139" priority="43" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="138" priority="44" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="45" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="136" priority="46" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q65">
-    <cfRule type="cellIs" dxfId="51" priority="211" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="212" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="213" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="214" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="135" priority="211" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="212" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="133" priority="213" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="214" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q66">
-    <cfRule type="cellIs" dxfId="47" priority="207" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="208" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="209" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="210" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="207" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="208" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="209" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="210" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q68">
-    <cfRule type="cellIs" dxfId="43" priority="280" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="281" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="282" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="283" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="127" priority="280" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="281" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="282" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="283" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17 Q28 Q31:Q33">
-    <cfRule type="cellIs" dxfId="39" priority="227" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="228" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="229" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="230" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="123" priority="227" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="228" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="121" priority="229" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="230" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q39">
-    <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="40" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="41" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="119" priority="39" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="40" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="117" priority="41" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="42" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q38">
-    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="36" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="115" priority="35" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="36" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="37" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="38" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q37">
-    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="32" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="33" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="31" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="32" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="109" priority="33" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="34" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q36">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="28" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="29" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="27" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="28" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="29" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q35">
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="23" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="24" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="25" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q46">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="15" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="16" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="17" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q40">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="12" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="13" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q41">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="8" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q48">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F53" sqref="F53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.21875" customWidth="1"/>
+    <col min="2" max="2" width="38.21875" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="45.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="8.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" style="2" customWidth="1"/>
+    <col min="6" max="9" width="8.77734375" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1"/>
+    <col min="11" max="11" width="47" bestFit="1" customWidth="1"/>
+    <col min="12" max="1005" width="8.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>12</v>
+      </c>
+      <c r="G2" s="6">
+        <v>4</v>
+      </c>
+      <c r="H2" s="6">
+        <v>8</v>
+      </c>
+      <c r="I2" s="6">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" ref="J2:J33" si="0">D2-SUM(F2:I2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3">
+        <v>64</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="6">
+        <v>32</v>
+      </c>
+      <c r="I3" s="6">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4">
+        <v>48</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="6">
+        <v>24</v>
+      </c>
+      <c r="I4" s="6">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5">
+        <v>32</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>20</v>
+      </c>
+      <c r="G5" s="6">
+        <v>12</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6">
+        <v>136</v>
+      </c>
+      <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6" s="6">
+        <v>64</v>
+      </c>
+      <c r="G6" s="6">
+        <v>40</v>
+      </c>
+      <c r="H6" s="6">
+        <v>4</v>
+      </c>
+      <c r="I6" s="6">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7">
+        <v>64</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8">
+        <v>1024</v>
+      </c>
+      <c r="E8">
+        <v>20480</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9">
+        <v>64</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>1024</v>
+      </c>
+      <c r="E10">
+        <v>22528</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="1">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>63</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>12</v>
+      </c>
+      <c r="G11" s="6">
+        <v>4</v>
+      </c>
+      <c r="H11" s="6">
+        <v>16</v>
+      </c>
+      <c r="I11" s="6">
+        <v>16</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>464</v>
+      </c>
+      <c r="E13">
+        <v>304</v>
+      </c>
+      <c r="F13" s="6">
+        <v>100</v>
+      </c>
+      <c r="G13" s="6">
+        <v>50</v>
+      </c>
+      <c r="H13" s="6">
+        <v>100</v>
+      </c>
+      <c r="I13" s="6">
+        <v>100</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14">
+        <v>142</v>
+      </c>
+      <c r="E14">
+        <v>160</v>
+      </c>
+      <c r="F14" s="6">
+        <v>64</v>
+      </c>
+      <c r="G14" s="6">
+        <v>32</v>
+      </c>
+      <c r="H14" s="6">
+        <v>20</v>
+      </c>
+      <c r="I14" s="6">
+        <v>16</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15">
+        <v>112</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15" s="6">
+        <v>50</v>
+      </c>
+      <c r="G15" s="6">
+        <v>16</v>
+      </c>
+      <c r="H15" s="6">
+        <v>20</v>
+      </c>
+      <c r="I15" s="6">
+        <v>16</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>32</v>
+      </c>
+      <c r="E16">
+        <v>120</v>
+      </c>
+      <c r="F16" s="6">
+        <v>4</v>
+      </c>
+      <c r="G16" s="6">
+        <v>4</v>
+      </c>
+      <c r="H16" s="6">
+        <v>12</v>
+      </c>
+      <c r="I16" s="6">
+        <v>12</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>153</v>
+      </c>
+      <c r="F17" s="6">
+        <v>3</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6">
+        <v>2</v>
+      </c>
+      <c r="I17" s="6">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6">
+        <v>3</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6">
+        <v>2</v>
+      </c>
+      <c r="I18" s="6">
+        <v>2</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19">
+        <v>4096</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="1">
+        <f t="shared" si="0"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20">
+        <v>32</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="6">
+        <v>8</v>
+      </c>
+      <c r="G20" s="6">
+        <v>4</v>
+      </c>
+      <c r="H20" s="6">
+        <v>8</v>
+      </c>
+      <c r="I20" s="6">
+        <v>8</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21">
+        <v>150</v>
+      </c>
+      <c r="E21">
+        <v>150</v>
+      </c>
+      <c r="F21" s="6">
+        <v>64</v>
+      </c>
+      <c r="G21" s="6">
+        <v>8</v>
+      </c>
+      <c r="H21" s="6">
+        <v>64</v>
+      </c>
+      <c r="I21" s="6">
+        <v>8</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23">
+        <v>1024</v>
+      </c>
+      <c r="E23">
+        <v>49152</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="1">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25">
+        <v>142</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25" s="6">
+        <v>64</v>
+      </c>
+      <c r="G25" s="6">
+        <v>32</v>
+      </c>
+      <c r="H25" s="6">
+        <v>20</v>
+      </c>
+      <c r="I25" s="6">
+        <v>16</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" s="6">
+        <v>2</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6">
+        <v>2</v>
+      </c>
+      <c r="I26" s="6">
+        <v>2</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27">
+        <v>112</v>
+      </c>
+      <c r="E27">
+        <v>8</v>
+      </c>
+      <c r="F27" s="6">
+        <v>50</v>
+      </c>
+      <c r="G27" s="6">
+        <v>16</v>
+      </c>
+      <c r="H27" s="6">
+        <v>20</v>
+      </c>
+      <c r="I27" s="6">
+        <v>16</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28">
+        <v>32</v>
+      </c>
+      <c r="E28">
+        <v>120</v>
+      </c>
+      <c r="F28" s="6">
+        <v>4</v>
+      </c>
+      <c r="G28" s="6">
+        <v>4</v>
+      </c>
+      <c r="H28" s="6">
+        <v>12</v>
+      </c>
+      <c r="I28" s="6">
+        <v>12</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29">
+        <v>7</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="6">
+        <v>3</v>
+      </c>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6">
+        <v>2</v>
+      </c>
+      <c r="I29" s="6">
+        <v>2</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30">
+        <v>240</v>
+      </c>
+      <c r="E30">
+        <v>16</v>
+      </c>
+      <c r="F30" s="6">
+        <v>80</v>
+      </c>
+      <c r="G30" s="6">
+        <v>30</v>
+      </c>
+      <c r="H30" s="6">
+        <v>50</v>
+      </c>
+      <c r="I30" s="6">
+        <v>50</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31">
+        <v>4592</v>
+      </c>
+      <c r="E31">
+        <v>16</v>
+      </c>
+      <c r="F31" s="6">
+        <v>1024</v>
+      </c>
+      <c r="G31" s="6">
+        <v>512</v>
+      </c>
+      <c r="H31" s="6">
+        <v>512</v>
+      </c>
+      <c r="I31" s="6">
+        <v>512</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="0"/>
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32">
+        <v>28</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="6">
+        <v>28</v>
+      </c>
+      <c r="I32" s="10"/>
+      <c r="J32" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33">
+        <v>28</v>
+      </c>
+      <c r="E33">
+        <v>36</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="6">
+        <v>28</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34">
+        <v>64</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" s="6">
+        <v>12</v>
+      </c>
+      <c r="G34" s="6">
+        <v>4</v>
+      </c>
+      <c r="H34" s="6">
+        <v>24</v>
+      </c>
+      <c r="I34" s="6">
+        <v>24</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" ref="J34:J54" si="1">D34-SUM(F34:I34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36">
+        <v>160</v>
+      </c>
+      <c r="E36">
+        <v>96</v>
+      </c>
+      <c r="F36" s="6">
+        <v>32</v>
+      </c>
+      <c r="G36" s="6">
+        <v>8</v>
+      </c>
+      <c r="H36" s="6">
+        <v>60</v>
+      </c>
+      <c r="I36" s="6">
+        <v>60</v>
+      </c>
+      <c r="J36" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37">
+        <v>46</v>
+      </c>
+      <c r="E37">
+        <v>50</v>
+      </c>
+      <c r="F37" s="6">
+        <v>14</v>
+      </c>
+      <c r="G37" s="6">
+        <v>4</v>
+      </c>
+      <c r="H37" s="6">
+        <v>14</v>
+      </c>
+      <c r="I37" s="6">
+        <v>14</v>
+      </c>
+      <c r="J37" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38">
+        <v>46</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" s="6">
+        <v>14</v>
+      </c>
+      <c r="G38" s="6">
+        <v>4</v>
+      </c>
+      <c r="H38" s="6">
+        <v>14</v>
+      </c>
+      <c r="I38" s="6">
+        <v>14</v>
+      </c>
+      <c r="J38" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>48</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6">
+        <v>2</v>
+      </c>
+      <c r="I39" s="6"/>
+      <c r="J39" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6">
+        <v>2</v>
+      </c>
+      <c r="I40" s="6"/>
+      <c r="J40" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41">
+        <v>4096</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="1">
+        <f t="shared" si="1"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42">
+        <v>32</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" s="6">
+        <v>8</v>
+      </c>
+      <c r="G42" s="6">
+        <v>4</v>
+      </c>
+      <c r="H42" s="6">
+        <v>8</v>
+      </c>
+      <c r="I42" s="6">
+        <v>8</v>
+      </c>
+      <c r="J42" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43">
+        <v>48</v>
+      </c>
+      <c r="E43">
+        <v>48</v>
+      </c>
+      <c r="F43" s="6">
+        <v>16</v>
+      </c>
+      <c r="G43" s="6">
+        <v>4</v>
+      </c>
+      <c r="H43" s="6">
+        <v>16</v>
+      </c>
+      <c r="I43" s="6">
+        <v>8</v>
+      </c>
+      <c r="J43" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45">
+        <v>256</v>
+      </c>
+      <c r="E45">
+        <v>56320</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="1">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K46" s="11"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47">
+        <v>46</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" s="6">
+        <v>14</v>
+      </c>
+      <c r="G47" s="6">
+        <v>4</v>
+      </c>
+      <c r="H47" s="6">
+        <v>14</v>
+      </c>
+      <c r="I47" s="6">
+        <v>14</v>
+      </c>
+      <c r="J47" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K47" s="11"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6">
+        <v>2</v>
+      </c>
+      <c r="I48" s="6"/>
+      <c r="J48" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49">
+        <v>46</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" s="6">
+        <v>14</v>
+      </c>
+      <c r="G49" s="6">
+        <v>4</v>
+      </c>
+      <c r="H49" s="6">
+        <v>14</v>
+      </c>
+      <c r="I49" s="6">
+        <v>14</v>
+      </c>
+      <c r="J49" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6">
+        <v>2</v>
+      </c>
+      <c r="I50" s="6"/>
+      <c r="J50" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51">
+        <v>248</v>
+      </c>
+      <c r="E51">
+        <v>8</v>
+      </c>
+      <c r="F51" s="6">
+        <v>80</v>
+      </c>
+      <c r="G51" s="6">
+        <v>30</v>
+      </c>
+      <c r="H51" s="6">
+        <v>50</v>
+      </c>
+      <c r="I51" s="6">
+        <v>50</v>
+      </c>
+      <c r="J51" s="1">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52">
+        <v>1528</v>
+      </c>
+      <c r="E52">
+        <v>16392</v>
+      </c>
+      <c r="F52" s="6">
+        <v>512</v>
+      </c>
+      <c r="G52" s="6">
+        <v>128</v>
+      </c>
+      <c r="H52" s="6">
+        <v>256</v>
+      </c>
+      <c r="I52" s="6">
+        <v>256</v>
+      </c>
+      <c r="J52" s="1">
+        <f t="shared" si="1"/>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B53" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53">
+        <v>40</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="1">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54">
+        <v>16</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" s="6">
+        <v>4</v>
+      </c>
+      <c r="G54" s="6">
+        <v>4</v>
+      </c>
+      <c r="H54" s="6">
+        <v>4</v>
+      </c>
+      <c r="I54" s="6">
+        <v>4</v>
+      </c>
+      <c r="J54" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J26">
+    <cfRule type="cellIs" dxfId="83" priority="81" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="82" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="84" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29">
+    <cfRule type="cellIs" dxfId="79" priority="77" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="78" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="79" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="80" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J30">
+    <cfRule type="cellIs" dxfId="75" priority="73" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="74" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="75" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="76" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J50">
+    <cfRule type="cellIs" dxfId="71" priority="61" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="62" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="63" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="64" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J44">
+    <cfRule type="cellIs" dxfId="67" priority="45" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="46" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="47" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="48" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J45">
+    <cfRule type="cellIs" dxfId="63" priority="49" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="50" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="51" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="52" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J47">
+    <cfRule type="cellIs" dxfId="59" priority="53" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="54" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="55" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="56" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J49">
+    <cfRule type="cellIs" dxfId="55" priority="57" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="58" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="59" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="60" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43">
+    <cfRule type="cellIs" dxfId="51" priority="41" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="42" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="43" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="44" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42">
+    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="38" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="39" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="40" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J54">
+    <cfRule type="cellIs" dxfId="43" priority="89" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="90" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="91" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="92" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17 J28 J31:J33">
+    <cfRule type="cellIs" dxfId="39" priority="85" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="86" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="87" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="88" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J39">
+    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="36" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J38">
+    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J37">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J35">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J46">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J48">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
SYSFW_RESASG: j721e: Update Resource Partitioning for Main R5FSS0
Ethernet firmware and PSDKRA will be combined into a single image
hence forward, leaving the Main R5FSS0 core1 free for customer.

To accomodate this, update the resource partitioning to combine
the resources from both for Main R5FSS0 core0 and leave a few resources
for Main R5FSS0 core1.

Signed-off-by: Nikhil Devshatwar <nikhil.nd@ti.com>
</commit_message>
<xml_diff>
--- a/respart/SYSFW-NAVSS-ResAssg.xlsx
+++ b/respart/SYSFW-NAVSS-ResAssg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11988" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11988" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="j721e" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="153">
   <si>
     <t>Resource</t>
   </si>
@@ -365,9 +365,6 @@
     <t>MCU Nav IA global events</t>
   </si>
   <si>
-    <t>MCU invalid flow OES</t>
-  </si>
-  <si>
     <t>Main Nav invalid flow OES</t>
   </si>
   <si>
@@ -478,13 +475,28 @@
   <si>
     <t>HOST_ID_R5_2
 (MCUSW)</t>
+  </si>
+  <si>
+    <t>MCU Nav GP Ring / Free Ring</t>
+  </si>
+  <si>
+    <t>MCU Nav invalid flow OES</t>
+  </si>
+  <si>
+    <t>MCU Nav Normal Capacity RX channel</t>
+  </si>
+  <si>
+    <t>MCU Nav Normal Capacity TX channel</t>
+  </si>
+  <si>
+    <t>Same as UDMA channel allocation, DO NOT modify here</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -536,6 +548,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -574,7 +593,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -610,6 +629,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -618,7 +646,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,6 +681,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2498,11 +2529,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -2529,10 +2560,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>3</v>
@@ -2571,7 +2602,7 @@
         <v>14</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -3082,17 +3113,17 @@
         <v>12</v>
       </c>
       <c r="O16" s="6">
+        <v>28</v>
+      </c>
+      <c r="P16" s="6">
         <v>8</v>
       </c>
-      <c r="P16" s="6">
-        <v>24</v>
-      </c>
       <c r="Q16" s="1">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>101</v>
       </c>
@@ -3136,17 +3167,17 @@
         <v>256</v>
       </c>
       <c r="O17" s="6">
+        <v>512</v>
+      </c>
+      <c r="P17" s="6">
         <v>256</v>
       </c>
-      <c r="P17" s="6">
-        <v>512</v>
-      </c>
       <c r="Q17" s="1">
         <f t="shared" si="1"/>
         <v>922</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>84</v>
       </c>
@@ -3190,17 +3221,17 @@
         <v>4</v>
       </c>
       <c r="O18" s="6">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="P18" s="6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q18" s="1">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>102</v>
       </c>
@@ -3232,7 +3263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>103</v>
       </c>
@@ -3276,17 +3307,17 @@
         <v>12</v>
       </c>
       <c r="O20" s="6">
+        <v>182</v>
+      </c>
+      <c r="P20" s="6">
         <v>40</v>
       </c>
-      <c r="P20" s="6">
-        <v>182</v>
-      </c>
       <c r="Q20" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>82</v>
       </c>
@@ -3302,45 +3333,59 @@
       <c r="E21" s="5">
         <v>316</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="14">
+        <f>F34</f>
         <v>36</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="14">
+        <f t="shared" ref="G21:P21" si="2">G34</f>
         <v>20</v>
       </c>
-      <c r="H21" s="6">
-        <v>2</v>
-      </c>
-      <c r="I21" s="6">
-        <v>2</v>
-      </c>
-      <c r="J21" s="6">
+      <c r="H21" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="I21" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J21" s="14">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="14">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="L21" s="6">
+      <c r="L21" s="14">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="14">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="N21" s="6">
+      <c r="N21" s="14">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="O21" s="6">
-        <v>7</v>
-      </c>
-      <c r="P21" s="6">
-        <v>15</v>
+      <c r="O21" s="14">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="P21" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="Q21" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R21" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>81</v>
       </c>
@@ -3356,45 +3401,59 @@
       <c r="E22" s="5">
         <v>16</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="14">
+        <f>F37</f>
         <v>36</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="14">
+        <f t="shared" ref="G22:P22" si="3">G37</f>
         <v>20</v>
       </c>
-      <c r="H22" s="6">
-        <v>2</v>
-      </c>
-      <c r="I22" s="6">
-        <v>2</v>
-      </c>
-      <c r="J22" s="6">
+      <c r="H22" s="14">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I22" s="14">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J22" s="14">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="K22" s="6">
+      <c r="K22" s="14">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L22" s="6">
+      <c r="L22" s="14">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M22" s="6">
+      <c r="M22" s="14">
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="N22" s="6">
+      <c r="N22" s="14">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="O22" s="6">
-        <v>7</v>
-      </c>
-      <c r="P22" s="6">
-        <v>8</v>
+      <c r="O22" s="14">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="P22" s="14">
+        <f t="shared" si="3"/>
+        <v>6</v>
       </c>
       <c r="Q22" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="R22" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>104</v>
       </c>
@@ -3410,31 +3469,59 @@
       <c r="E23" s="5">
         <v>140</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6">
+      <c r="F23" s="14">
+        <f t="shared" ref="F23:P23" si="4">F38</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="14">
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="M23" s="6">
+      <c r="M23" s="14">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="N23" s="6">
+      <c r="N23" s="14">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6">
+      <c r="O23" s="14">
+        <f>O38</f>
         <v>132</v>
       </c>
+      <c r="P23" s="14">
+        <f t="shared" ref="P23" si="5">P38</f>
+        <v>0</v>
+      </c>
       <c r="Q23" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R23" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>80</v>
       </c>
@@ -3450,29 +3537,59 @@
       <c r="E24" s="5">
         <v>304</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="14">
+        <f>F35</f>
         <v>4</v>
       </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6">
-        <v>2</v>
-      </c>
-      <c r="P24" s="6">
-        <v>4</v>
+      <c r="G24" s="14">
+        <f t="shared" ref="G24:P24" si="6">G35</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="14">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="P24" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="Q24" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R24" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>78</v>
       </c>
@@ -3488,27 +3605,59 @@
       <c r="E25" s="5">
         <v>300</v>
       </c>
-      <c r="F25" s="6">
-        <v>2</v>
-      </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6">
-        <v>2</v>
+      <c r="F25" s="14">
+        <f>F36</f>
+        <v>2</v>
+      </c>
+      <c r="G25" s="14">
+        <f t="shared" ref="G25:P25" si="7">G36</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="14">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="P25" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="Q25" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R25" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>79</v>
       </c>
@@ -3524,29 +3673,59 @@
       <c r="E26" s="5">
         <v>4</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="14">
+        <f>F39</f>
         <v>4</v>
       </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6">
-        <v>2</v>
-      </c>
-      <c r="P26" s="6">
-        <v>4</v>
+      <c r="G26" s="14">
+        <f t="shared" ref="G26:P26" si="8">G39</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="14">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="P26" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="Q26" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R26" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>77</v>
       </c>
@@ -3562,27 +3741,59 @@
       <c r="E27" s="5">
         <v>0</v>
       </c>
-      <c r="F27" s="6">
-        <v>2</v>
-      </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6">
-        <v>2</v>
+      <c r="F27" s="14">
+        <f>F40</f>
+        <v>2</v>
+      </c>
+      <c r="G27" s="14">
+        <f t="shared" ref="G27:P27" si="9">G40</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="14">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="P27" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="Q27" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R27" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>105</v>
       </c>
@@ -3614,7 +3825,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>83</v>
       </c>
@@ -3668,7 +3879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>85</v>
       </c>
@@ -3698,19 +3909,19 @@
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="P30" s="6">
         <v>8</v>
       </c>
       <c r="Q30" s="1">
         <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>15</v>
@@ -3740,7 +3951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>107</v>
       </c>
@@ -3848,10 +4059,10 @@
         <v>8</v>
       </c>
       <c r="O34" s="6">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="P34" s="6">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="Q34" s="1">
         <f t="shared" si="1"/>
@@ -3886,11 +4097,9 @@
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6">
-        <v>2</v>
-      </c>
-      <c r="P35" s="6">
-        <v>4</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="P35" s="6"/>
       <c r="Q35" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -3923,10 +4132,10 @@
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6">
-        <v>2</v>
-      </c>
+      <c r="O36" s="6">
+        <v>2</v>
+      </c>
+      <c r="P36" s="6"/>
       <c r="Q36" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3976,14 +4185,14 @@
         <v>8</v>
       </c>
       <c r="O37" s="6">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="P37" s="6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q37" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
@@ -4017,10 +4226,10 @@
       <c r="N38" s="6">
         <v>6</v>
       </c>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6">
+      <c r="O38" s="6">
         <v>132</v>
       </c>
+      <c r="P38" s="6"/>
       <c r="Q38" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4054,11 +4263,9 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
       <c r="O39" s="6">
-        <v>2</v>
-      </c>
-      <c r="P39" s="6">
-        <v>4</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="P39" s="6"/>
       <c r="Q39" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4091,10 +4298,10 @@
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6">
-        <v>2</v>
-      </c>
+      <c r="O40" s="6">
+        <v>2</v>
+      </c>
+      <c r="P40" s="6"/>
       <c r="Q40" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4310,7 +4517,7 @@
         <v>0</v>
       </c>
       <c r="R46" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
@@ -4351,7 +4558,7 @@
         <v>104</v>
       </c>
       <c r="R47" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
@@ -4398,17 +4605,17 @@
         <v>8</v>
       </c>
       <c r="O48" s="6">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="P48" s="6">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="Q48" s="1">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>111</v>
       </c>
@@ -4462,7 +4669,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
         <v>68</v>
       </c>
@@ -4506,19 +4713,19 @@
         <v>4</v>
       </c>
       <c r="O50" s="6">
+        <v>16</v>
+      </c>
+      <c r="P50" s="6">
         <v>4</v>
       </c>
-      <c r="P50" s="6">
-        <v>16</v>
-      </c>
       <c r="Q50" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>40</v>
@@ -4548,9 +4755,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>70</v>
+        <v>148</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>40</v>
@@ -4601,10 +4808,11 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R52" s="11"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>40</v>
@@ -4618,47 +4826,51 @@
       <c r="E53" s="5">
         <v>50</v>
       </c>
-      <c r="F53" s="6">
+      <c r="F53" s="14">
+        <f>F63</f>
         <v>12</v>
       </c>
-      <c r="G53" s="6">
+      <c r="G53" s="14">
         <v>6</v>
       </c>
-      <c r="H53" s="6">
+      <c r="H53" s="14">
         <v>5</v>
       </c>
-      <c r="I53" s="6">
-        <v>2</v>
-      </c>
-      <c r="J53" s="6">
-        <v>2</v>
-      </c>
-      <c r="K53" s="6">
-        <v>2</v>
-      </c>
-      <c r="L53" s="6">
-        <v>2</v>
-      </c>
-      <c r="M53" s="6">
-        <v>2</v>
-      </c>
-      <c r="N53" s="6">
-        <v>2</v>
-      </c>
-      <c r="O53" s="6">
+      <c r="I53" s="14">
+        <v>2</v>
+      </c>
+      <c r="J53" s="14">
+        <v>2</v>
+      </c>
+      <c r="K53" s="14">
+        <v>2</v>
+      </c>
+      <c r="L53" s="14">
+        <v>2</v>
+      </c>
+      <c r="M53" s="14">
+        <v>2</v>
+      </c>
+      <c r="N53" s="14">
+        <v>2</v>
+      </c>
+      <c r="O53" s="14">
         <v>3</v>
       </c>
-      <c r="P53" s="6">
+      <c r="P53" s="14">
         <v>2</v>
       </c>
       <c r="Q53" s="1">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R53" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>40</v>
@@ -4672,45 +4884,49 @@
       <c r="E54" s="5">
         <v>2</v>
       </c>
-      <c r="F54" s="6">
+      <c r="F54" s="14">
+        <f>F65</f>
         <v>12</v>
       </c>
-      <c r="G54" s="6">
+      <c r="G54" s="14">
         <v>6</v>
       </c>
-      <c r="H54" s="6">
+      <c r="H54" s="14">
         <v>5</v>
       </c>
-      <c r="I54" s="6">
-        <v>2</v>
-      </c>
-      <c r="J54" s="6">
-        <v>2</v>
-      </c>
-      <c r="K54" s="6">
-        <v>2</v>
-      </c>
-      <c r="L54" s="6">
-        <v>2</v>
-      </c>
-      <c r="M54" s="6">
-        <v>2</v>
-      </c>
-      <c r="N54" s="6">
-        <v>2</v>
-      </c>
-      <c r="O54" s="6">
+      <c r="I54" s="14">
+        <v>2</v>
+      </c>
+      <c r="J54" s="14">
+        <v>2</v>
+      </c>
+      <c r="K54" s="14">
+        <v>2</v>
+      </c>
+      <c r="L54" s="14">
+        <v>2</v>
+      </c>
+      <c r="M54" s="14">
+        <v>2</v>
+      </c>
+      <c r="N54" s="14">
+        <v>2</v>
+      </c>
+      <c r="O54" s="14">
         <v>3</v>
       </c>
-      <c r="P54" s="6">
+      <c r="P54" s="14">
         <v>2</v>
       </c>
       <c r="Q54" s="1">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R54" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>66</v>
       </c>
@@ -4726,25 +4942,28 @@
       <c r="E55" s="5">
         <v>48</v>
       </c>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6">
-        <v>2</v>
-      </c>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="6"/>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
-      <c r="P55" s="6"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14">
+        <v>2</v>
+      </c>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="14"/>
+      <c r="P55" s="14"/>
       <c r="Q55" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R55" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>65</v>
       </c>
@@ -4760,25 +4979,28 @@
       <c r="E56" s="5">
         <v>0</v>
       </c>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6">
-        <v>2</v>
-      </c>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="6"/>
-      <c r="O56" s="6"/>
-      <c r="P56" s="6"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14">
+        <v>2</v>
+      </c>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="14"/>
+      <c r="N56" s="14"/>
+      <c r="O56" s="14"/>
+      <c r="P56" s="14"/>
       <c r="Q56" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R56" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>105</v>
       </c>
@@ -4810,7 +5032,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>67</v>
       </c>
@@ -4864,7 +5086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>69</v>
       </c>
@@ -4912,9 +5134,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>39</v>
@@ -4944,9 +5166,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>39</v>
@@ -4976,9 +5198,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>39</v>
@@ -5008,9 +5230,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>39</v>
@@ -5062,7 +5284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
         <v>64</v>
       </c>
@@ -5098,7 +5320,7 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>39</v>
@@ -5186,7 +5408,7 @@
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>55</v>
@@ -5220,7 +5442,7 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>55</v>
@@ -5248,7 +5470,7 @@
       <c r="O68" s="10"/>
       <c r="P68" s="6"/>
       <c r="Q68" s="1">
-        <f t="shared" ref="Q68" si="2">D68-SUM(F68:P68)</f>
+        <f t="shared" ref="Q68" si="10">D68-SUM(F68:P68)</f>
         <v>0</v>
       </c>
     </row>
@@ -5584,11 +5806,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F53" sqref="F53"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -5615,28 +5837,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>121</v>
-      </c>
       <c r="F1" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>14</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -5644,7 +5866,7 @@
         <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -5677,7 +5899,7 @@
         <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
@@ -5706,7 +5928,7 @@
         <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
@@ -5735,7 +5957,7 @@
         <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
@@ -5764,7 +5986,7 @@
         <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
         <v>44</v>
@@ -5797,7 +6019,7 @@
         <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -5822,7 +6044,7 @@
         <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
@@ -5847,7 +6069,7 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
@@ -5872,7 +6094,7 @@
         <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -5897,7 +6119,7 @@
         <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -5930,7 +6152,7 @@
         <v>102</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" t="s">
         <v>58</v>
@@ -5955,7 +6177,7 @@
         <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
         <v>31</v>
@@ -5988,7 +6210,7 @@
         <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
         <v>29</v>
@@ -6021,7 +6243,7 @@
         <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
@@ -6054,7 +6276,7 @@
         <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
         <v>30</v>
@@ -6087,7 +6309,7 @@
         <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -6118,7 +6340,7 @@
         <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -6149,7 +6371,7 @@
         <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
         <v>59</v>
@@ -6174,7 +6396,7 @@
         <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C20" t="s">
         <v>32</v>
@@ -6207,7 +6429,7 @@
         <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s">
         <v>35</v>
@@ -6237,10 +6459,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C22" t="s">
         <v>60</v>
@@ -6265,7 +6487,7 @@
         <v>107</v>
       </c>
       <c r="B23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C23" t="s">
         <v>61</v>
@@ -6290,7 +6512,7 @@
         <v>106</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" t="s">
         <v>62</v>
@@ -6315,7 +6537,7 @@
         <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
@@ -6348,7 +6570,7 @@
         <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C26" t="s">
         <v>19</v>
@@ -6379,7 +6601,7 @@
         <v>109</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
         <v>20</v>
@@ -6412,7 +6634,7 @@
         <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C28" t="s">
         <v>22</v>
@@ -6445,7 +6667,7 @@
         <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
@@ -6476,7 +6698,7 @@
         <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C30" t="s">
         <v>37</v>
@@ -6509,7 +6731,7 @@
         <v>101</v>
       </c>
       <c r="B31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
@@ -6539,10 +6761,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C32" t="s">
         <v>44</v>
@@ -6566,10 +6788,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
         <v>44</v>
@@ -6596,7 +6818,7 @@
         <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
@@ -6626,10 +6848,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C35" t="s">
         <v>58</v>
@@ -6654,7 +6876,7 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C36" t="s">
         <v>31</v>
@@ -6684,10 +6906,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C37" t="s">
         <v>29</v>
@@ -6717,10 +6939,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C38" t="s">
         <v>28</v>
@@ -6753,7 +6975,7 @@
         <v>66</v>
       </c>
       <c r="B39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C39" t="s">
         <v>27</v>
@@ -6780,7 +7002,7 @@
         <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C40" t="s">
         <v>26</v>
@@ -6807,7 +7029,7 @@
         <v>105</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C41" t="s">
         <v>59</v>
@@ -6832,7 +7054,7 @@
         <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C42" t="s">
         <v>32</v>
@@ -6865,7 +7087,7 @@
         <v>69</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C43" t="s">
         <v>35</v>
@@ -6895,10 +7117,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C44" t="s">
         <v>60</v>
@@ -6920,10 +7142,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C45" t="s">
         <v>61</v>
@@ -6945,10 +7167,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C46" t="s">
         <v>62</v>
@@ -6971,10 +7193,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C47" t="s">
         <v>21</v>
@@ -7008,7 +7230,7 @@
         <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C48" t="s">
         <v>19</v>
@@ -7032,10 +7254,10 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C49" t="s">
         <v>20</v>
@@ -7068,7 +7290,7 @@
         <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C50" t="s">
         <v>18</v>
@@ -7095,7 +7317,7 @@
         <v>71</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C51" t="s">
         <v>37</v>
@@ -7128,7 +7350,7 @@
         <v>111</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C52" t="s">
         <v>38</v>
@@ -7161,7 +7383,7 @@
         <v>95</v>
       </c>
       <c r="B53" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C53" t="s">
         <v>44</v>
@@ -7186,7 +7408,7 @@
         <v>96</v>
       </c>
       <c r="B54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C54" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
SYSFW-NAVSS-ResAssg: j721e: Allocate the flows for ethfw to ALL
Ethernet firmware uses a client server model where it owns a chunk
of 64 flows and dynamically assigns few of these to the clients.

Till the flow sharing support is available, mark these resources
as HOST_ID_ALL

Signed-off-by: Nikhil Devshatwar <nikhil.nd@ti.com>
</commit_message>
<xml_diff>
--- a/respart/SYSFW-NAVSS-ResAssg.xlsx
+++ b/respart/SYSFW-NAVSS-ResAssg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11988" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11988" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="j721e" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="154">
   <si>
     <t>Resource</t>
   </si>
@@ -490,6 +490,10 @@
   </si>
   <si>
     <t>Same as UDMA channel allocation, DO NOT modify here</t>
+  </si>
+  <si>
+    <t>Ideally 72 for R50_0 and 8 for R50_1
+For flow sharing purpose, mark them as host_id_all</t>
   </si>
 </sst>
 </file>
@@ -646,7 +650,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -685,6 +689,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2529,11 +2536,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -3470,7 +3477,7 @@
         <v>140</v>
       </c>
       <c r="F23" s="14">
-        <f t="shared" ref="F23:P23" si="4">F38</f>
+        <f t="shared" ref="F23:N23" si="4">F38</f>
         <v>0</v>
       </c>
       <c r="G23" s="14">
@@ -3879,7 +3886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>85</v>
       </c>
@@ -3908,15 +3915,14 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
-      <c r="O30" s="6">
-        <v>72</v>
-      </c>
-      <c r="P30" s="6">
-        <v>8</v>
-      </c>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
       <c r="Q30" s="1">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>128</v>
+      </c>
+      <c r="R30" s="15" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -5806,19 +5812,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36.21875" customWidth="1"/>
-    <col min="2" max="2" width="38.21875" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="45.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="8.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38.21875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="45.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="8.6640625" style="2" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11.77734375" style="2" customWidth="1"/>
     <col min="6" max="9" width="8.77734375" customWidth="1"/>
     <col min="10" max="10" width="12.109375" customWidth="1"/>
@@ -6221,16 +6227,20 @@
       <c r="E14">
         <v>160</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="14">
+        <f>F25</f>
         <v>64</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="14">
+        <f t="shared" ref="G14:I14" si="1">G25</f>
         <v>32</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="14">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="14">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="J14" s="1">
@@ -6254,16 +6264,20 @@
       <c r="E15">
         <v>8</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="14">
+        <f>F27</f>
         <v>50</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="14">
+        <f>G27</f>
         <v>16</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="14">
+        <f>H27</f>
         <v>20</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="14">
+        <f>I27</f>
         <v>16</v>
       </c>
       <c r="J15" s="1">
@@ -6287,16 +6301,20 @@
       <c r="E16">
         <v>120</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="14">
+        <f>F28</f>
         <v>4</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="14">
+        <f>G28</f>
         <v>4</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="14">
+        <f>H28</f>
         <v>12</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="14">
+        <f>I28</f>
         <v>12</v>
       </c>
       <c r="J16" s="1">
@@ -6320,19 +6338,25 @@
       <c r="E17">
         <v>153</v>
       </c>
-      <c r="F17" s="6">
-        <v>3</v>
-      </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6">
-        <v>2</v>
-      </c>
-      <c r="I17" s="6">
+      <c r="F17" s="14">
+        <f>F26</f>
+        <v>2</v>
+      </c>
+      <c r="G17" s="14">
+        <f>G26</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="14">
+        <f>H26</f>
+        <v>2</v>
+      </c>
+      <c r="I17" s="14">
+        <f>I26</f>
         <v>2</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -6351,14 +6375,20 @@
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="14">
+        <f>F29</f>
         <v>3</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6">
-        <v>2</v>
-      </c>
-      <c r="I18" s="6">
+      <c r="G18" s="14">
+        <f>G29</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="14">
+        <f>H29</f>
+        <v>2</v>
+      </c>
+      <c r="I18" s="14">
+        <f>I29</f>
         <v>2</v>
       </c>
       <c r="J18" s="1">
@@ -6842,7 +6872,7 @@
         <v>24</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" ref="J34:J54" si="1">D34-SUM(F34:I34)</f>
+        <f t="shared" ref="J34:J54" si="2">D34-SUM(F34:I34)</f>
         <v>0</v>
       </c>
     </row>
@@ -6867,7 +6897,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6900,7 +6930,7 @@
         <v>60</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6920,20 +6950,24 @@
       <c r="E37">
         <v>50</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="14">
+        <f>F47</f>
         <v>14</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G37" s="14">
+        <f>G47</f>
         <v>4</v>
       </c>
-      <c r="H37" s="6">
+      <c r="H37" s="14">
+        <f>H47</f>
         <v>14</v>
       </c>
-      <c r="I37" s="6">
+      <c r="I37" s="14">
+        <f>I47</f>
         <v>14</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6953,20 +6987,24 @@
       <c r="E38">
         <v>2</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="14">
+        <f>F49</f>
         <v>14</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="14">
+        <f>G49</f>
         <v>4</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H38" s="14">
+        <f>H49</f>
         <v>14</v>
       </c>
-      <c r="I38" s="6">
+      <c r="I38" s="14">
+        <f>I49</f>
         <v>14</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6986,14 +7024,24 @@
       <c r="E39">
         <v>48</v>
       </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6">
-        <v>2</v>
-      </c>
-      <c r="I39" s="6"/>
+      <c r="F39" s="14">
+        <f>F48</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="14">
+        <f>G48</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="14">
+        <f>H48</f>
+        <v>2</v>
+      </c>
+      <c r="I39" s="14">
+        <f>I48</f>
+        <v>0</v>
+      </c>
       <c r="J39" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7013,14 +7061,24 @@
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6">
-        <v>2</v>
-      </c>
-      <c r="I40" s="6"/>
+      <c r="F40" s="14">
+        <f>F50</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="14">
+        <f>G50</f>
+        <v>0</v>
+      </c>
+      <c r="H40" s="14">
+        <f>H50</f>
+        <v>2</v>
+      </c>
+      <c r="I40" s="14">
+        <f>I50</f>
+        <v>0</v>
+      </c>
       <c r="J40" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7045,7 +7103,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
       <c r="J41" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4096</v>
       </c>
     </row>
@@ -7078,7 +7136,7 @@
         <v>8</v>
       </c>
       <c r="J42" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -7111,7 +7169,7 @@
         <v>8</v>
       </c>
       <c r="J43" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -7136,7 +7194,7 @@
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
       <c r="J44" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -7161,7 +7219,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
       <c r="J45" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
     </row>
@@ -7186,7 +7244,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
       <c r="J46" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K46" s="11"/>
@@ -7220,7 +7278,7 @@
         <v>14</v>
       </c>
       <c r="J47" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K47" s="11"/>
@@ -7248,7 +7306,7 @@
       </c>
       <c r="I48" s="6"/>
       <c r="J48" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7281,7 +7339,7 @@
         <v>14</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7308,7 +7366,7 @@
       </c>
       <c r="I50" s="6"/>
       <c r="J50" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7341,7 +7399,7 @@
         <v>50</v>
       </c>
       <c r="J51" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
     </row>
@@ -7374,7 +7432,7 @@
         <v>256</v>
       </c>
       <c r="J52" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>376</v>
       </c>
     </row>
@@ -7399,7 +7457,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
       <c r="J53" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
@@ -7432,7 +7490,7 @@
         <v>4</v>
       </c>
       <c r="J54" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SYSFW-NAVSS-ResAssg: am6x: Update the rsource count for Main NAV rings
SYSFW documentation for am6x says for Main NAVSS
Only 1 RX ring is reserved but 2 RX channels are reserved
This is not consistent.

Fix this manually by updating the resource count and start value.

Signed-off-by: Nikhil Devshatwar <nikhil.nd@ti.com>
</commit_message>
<xml_diff>
--- a/respart/SYSFW-NAVSS-ResAssg.xlsx
+++ b/respart/SYSFW-NAVSS-ResAssg.xlsx
@@ -5813,10 +5813,10 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H38" sqref="H38"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -6265,19 +6265,19 @@
         <v>8</v>
       </c>
       <c r="F15" s="14">
-        <f>F27</f>
+        <f t="shared" ref="F15:I16" si="2">F27</f>
         <v>50</v>
       </c>
       <c r="G15" s="14">
-        <f>G27</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="H15" s="14">
-        <f>H27</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="I15" s="14">
-        <f>I27</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J15" s="1">
@@ -6302,19 +6302,19 @@
         <v>120</v>
       </c>
       <c r="F16" s="14">
-        <f>F28</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="G16" s="14">
-        <f>G28</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H16" s="14">
-        <f>H28</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="I16" s="14">
-        <f>I28</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J16" s="1">
@@ -6333,10 +6333,10 @@
         <v>27</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F17" s="14">
         <f>F26</f>
@@ -6356,7 +6356,7 @@
       </c>
       <c r="J17" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -6872,7 +6872,7 @@
         <v>24</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" ref="J34:J54" si="2">D34-SUM(F34:I34)</f>
+        <f t="shared" ref="J34:J54" si="3">D34-SUM(F34:I34)</f>
         <v>0</v>
       </c>
     </row>
@@ -6897,7 +6897,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6930,7 +6930,7 @@
         <v>60</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6967,7 +6967,7 @@
         <v>14</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7004,7 +7004,7 @@
         <v>14</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7041,7 +7041,7 @@
         <v>0</v>
       </c>
       <c r="J39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7078,7 +7078,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7103,7 +7103,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
       <c r="J41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4096</v>
       </c>
     </row>
@@ -7136,7 +7136,7 @@
         <v>8</v>
       </c>
       <c r="J42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
@@ -7169,7 +7169,7 @@
         <v>8</v>
       </c>
       <c r="J43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
@@ -7194,7 +7194,7 @@
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
       <c r="J44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7219,7 +7219,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
       <c r="J45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>256</v>
       </c>
     </row>
@@ -7244,7 +7244,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
       <c r="J46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K46" s="11"/>
@@ -7278,7 +7278,7 @@
         <v>14</v>
       </c>
       <c r="J47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K47" s="11"/>
@@ -7306,7 +7306,7 @@
       </c>
       <c r="I48" s="6"/>
       <c r="J48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7339,7 +7339,7 @@
         <v>14</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7366,7 +7366,7 @@
       </c>
       <c r="I50" s="6"/>
       <c r="J50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7399,7 +7399,7 @@
         <v>50</v>
       </c>
       <c r="J51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
     </row>
@@ -7432,7 +7432,7 @@
         <v>256</v>
       </c>
       <c r="J52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>376</v>
       </c>
     </row>
@@ -7457,7 +7457,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
       <c r="J53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
     </row>
@@ -7490,7 +7490,7 @@
         <v>4</v>
       </c>
       <c r="J54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>